<commit_message>
list of documents 2012
</commit_message>
<xml_diff>
--- a/aakash_documents_list.xlsx
+++ b/aakash_documents_list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="320">
   <si>
     <t>Date</t>
   </si>
@@ -459,6 +459,522 @@
   </si>
   <si>
     <t>DataWind, the Canadian company that is manufacturing Aakash, has started the online booking and pre booking of the much anticipated low cost Android tablet. Online booking is for students' version of the tablet and pre booking is for UbiSlate 7, the upgraded version of Aakash. Students' version of Aakash will be available for Rs 2,500 and will be delivered in seven days. The commercial version, UbiSlate 7 is priced at Rs 2,999. The payment mode for both the tablets is cash on delivery.</t>
+  </si>
+  <si>
+    <t>03/01/2012</t>
+  </si>
+  <si>
+    <t>14 Lakh Aakash Tablets Booked in 14 Days</t>
+  </si>
+  <si>
+    <t>Harsimran Julka, The Economic Times</t>
+  </si>
+  <si>
+    <t>http://articles.economictimes.indiatimes.com/2012-01-03/news/30584606_1_aakash-tablets-indian-tablet-market-current-tablet</t>
+  </si>
+  <si>
+    <t>To cater to the 'unexpected' demand, UK-based vendor Datawind, the maker of the $35 tablet, has decided to establish three new factories - in Cochin, Noida and Hyderabad - in the first half of 2012 to assemble the tablet. Datawind currently has only one factory in Hyderabad, with its vendor Quad, which makes the LCD panel for the tablet.</t>
+  </si>
+  <si>
+    <t>08/01/2012</t>
+  </si>
+  <si>
+    <t>Kapil Sibal's Cheap Aakash Proves to be a Dud</t>
+  </si>
+  <si>
+    <t>Ritika Chopra, Mail Today</t>
+  </si>
+  <si>
+    <t>http://indiatoday.intoday.in/story/kapil-sibal-cheapest-tablet-of-world-aakash-failure/1/167730.html</t>
+  </si>
+  <si>
+    <t>Three months after it was launched amid much fanfare, Aakash - an affordable "access device" priced at Rs.2,250 - seems to be in need of a makeover. The feedback received from 600-odd students, who have used the tablet as part of the pilot run, has revealed quite a few drawbacks in the device that have been acknowledged by Kapil Sibal's Ministry of Human Resource Development (HRD) and are currently being worked upon.</t>
+  </si>
+  <si>
+    <t>13/01/2012</t>
+  </si>
+  <si>
+    <t>Kapil Sibal's Low-Cost Aakash Tablet may be Shelved </t>
+  </si>
+  <si>
+    <t>Sanjay Singh, Mail Today</t>
+  </si>
+  <si>
+    <t>http://indiatoday.intoday.in/story/aakash-low-cost-india-tablet-kapil-sibal/1/168564.html</t>
+  </si>
+  <si>
+    <t>The Union human resource development (HRD) ministry may refuse to extend the letter of credit (LC) to Montreal-based DataWind, the makers of the world's cheapest computer tablet, Aakash, priced at Rs.2,250 after a series of faults were detected, owing to which buyers have largely dumped it... Sources said the idea conceptualised by Sibal for an affordable tablet has been hijacked by corporate giant, Mukesh-Ambani's Reliance Industries Ltd (RIL), which plans to launch its fourthgeneration (4G) services later this year and sell tablets at cheap price of around Rs.3,500.</t>
+  </si>
+  <si>
+    <t>16/01/2012</t>
+  </si>
+  <si>
+    <t>Aakash Tablet: Datawind Opposes IIT's Test Standard</t>
+  </si>
+  <si>
+    <t>The Times of India</t>
+  </si>
+  <si>
+    <t>http://timesofindia.indiatimes.com/tech/tech-news/Aakash-tablet-Datawind-opposes-IITs-test-standard/articleshow/11508146.cms</t>
+  </si>
+  <si>
+    <t>Datawind CEO Sunit Sing Tuli told PTI that the test specifications have been proposed by the IIT after the tender document was submitted and were not a part of the original tender... Test criteria made by the IIT is based on millitary specification of a rugged product, he said, adding, "We have objected to it that millitary specifications do not make sense."</t>
+  </si>
+  <si>
+    <t>18/01/2012</t>
+  </si>
+  <si>
+    <t>Aakash Loses Government Edge</t>
+  </si>
+  <si>
+    <t>http://www.themobileindian.com/news/4811_Aakash-loses-government-edge</t>
+  </si>
+  <si>
+    <t>Aakash tablet has been criticised for its poor battery life, poor processor that is unable to do multi-tasking and below par display quality. Meanwhile, the Indian government is now thinking to bring a better low cost tablet which will address the drawback of the original Aakash tablet.</t>
+  </si>
+  <si>
+    <t>01/02/2012</t>
+  </si>
+  <si>
+    <t>Searching for the Aakash</t>
+  </si>
+  <si>
+    <t>Jairaj Bhattacharya, Chiteisri Devi, and Kenneth R. Foster, IEEE Spectrum</t>
+  </si>
+  <si>
+    <t>http://spectrum.ieee.org/geek-life/tools-toys/searching-for-the-aakash</t>
+  </si>
+  <si>
+    <t>Aakash-1 is a basic 7-inch tablet running Android 2.2 on a 366-megahertz Conexant processor with a microSD slot, two standard USB ports, an audio port and input jack, and a mere 256 megabytes of memory. It has Wi-Fi connectivity but no Bluetooth or cellular service. The key word is basic—and painfully slow. Slower even than cheap mobile phones in India, which typically come with 699‑MHz processors. Its limited battery life—a maximum of 2.5 hours, which falls to 1 hour and 20 minutes with video or other applications running—is disappointing for a device that’s supposed to be used in villages where access to electricity is sporadic at best.</t>
+  </si>
+  <si>
+    <t>02/02/2012</t>
+  </si>
+  <si>
+    <t>Govt to Take away Aakash Deal from IIT Rajasthan </t>
+  </si>
+  <si>
+    <t>The Economic Times</t>
+  </si>
+  <si>
+    <t>http://articles.economictimes.indiatimes.com/2012-02-02/news/31017361_1_aakash2-iit-rajasthan-tablets</t>
+  </si>
+  <si>
+    <t>The government has decided to take future tendering and procurement for Aakash2 tablets from IIT Rajasthan, and hand it over to public sector undertakings. The decision comes in the wake of a spat between IIT-Rajasthan, current procurement agency for Aakash and the tablet's current maker Datawind, which has led to a stoppage of supplies. "We have realised that educational institutes are not capable of handling tenders as it involves large sums of money and handling vendors. Public sector undertakings are much better equipped to handle it," said a government official, involved with [NMEICT].</t>
+  </si>
+  <si>
+    <t>03/02/2012</t>
+  </si>
+  <si>
+    <t>Aakash Tablet: 3 More IITs to Work for Making it Cheaper</t>
+  </si>
+  <si>
+    <t>Kanchana Devi, Truthdive</t>
+  </si>
+  <si>
+    <t>http://truthdive.com/2012/02/03/aakash-tablet-3-more-iits-to-work-for-making-it-cheaper.html</t>
+  </si>
+  <si>
+    <t>Apart from IIT Rajasthan, which is spearheading the project, IIT Mumbai, IIT Madras and IIT Kanpur would also be roped in for the project, sources in the HRD Ministry said... Several PSUs and Centre for Development of Advanced Computing are also expected to chip in to roll out the second phase of the Aakash. The speed of the device will come at 800 MHz instead of 300 MHz at present. The HRD ministry, which has developed prototype of Aakash, also wants the public sector Indian Telephone Industries (ITI) to participate in the bid to supply Aakash 2 tablets from April this year.</t>
+  </si>
+  <si>
+    <t>08/02/2012</t>
+  </si>
+  <si>
+    <t>Aakash Lurches toward Another Crisis as India Loses Patience with DataWind</t>
+  </si>
+  <si>
+    <t>Daniel Cooper, Engadget</t>
+  </si>
+  <si>
+    <t>http://www.engadget.com/2012/02/22/aakash-stalls/</t>
+  </si>
+  <si>
+    <t>Despite a record-breaking 1.4 million pre-orders gained in under a fortnight, maker DataWind has only shipped 10,000 units to nearly universal derision. Early adopters have found the processor too slow, battery life too short and the resistive touchscreen difficult to use. Kapil Sibal's Human Resource Development ministry now plans to re-open tendering for a replacement contractor and withdraw DataWind's deal for a further 90,000 units.</t>
+  </si>
+  <si>
+    <t>14/02/2012</t>
+  </si>
+  <si>
+    <t>Clouds of Doubt over Aakash</t>
+  </si>
+  <si>
+    <t>Arun Nigavekar, Financial Chronicle</t>
+  </si>
+  <si>
+    <t>http://www.mydigitalfc.com/op-ed/clouds-doubt-over-aakash-680</t>
+  </si>
+  <si>
+    <t>It seems that the government is unhappy with the company [Datawind] after various faults were detected in the Aakash tablet. The HRD ministry now desires that the devise is made more indigenous and the price should further reduce. IIT Mumbai and IIT Kanpur are likely to be involved to address these aspects. It is also reported that PSUs such as ITI or Telecommunications Consultants India (TCIL) are being considered for procurement of Aakash 2 tablets. Moreover, IIT Rajasthan will be no more involved in the drafting of specifications and features of the Aakash 2 tablets. It will be taken care by the department of IT, ministry of communications and IT. A special committee headed by the IT ministry is going to decide over the future specifications of the Aakash 2 tablets.</t>
+  </si>
+  <si>
+    <t>21/02/2012</t>
+  </si>
+  <si>
+    <t>Aakash Tablet Project - Govt Dumps Datawind; MediaNama’s RTI</t>
+  </si>
+  <si>
+    <t>Vikas SN, MediaNama</t>
+  </si>
+  <si>
+    <t>http://www.medianama.com/2012/02/223-aakash-tablet-project-govt-dumps-datawind-medianamas-rti/</t>
+  </si>
+  <si>
+    <t>Quoting two unnamed senior government officials, the report states that the government is now planning to launch a revamped tablet at the same price tag. The tablet will apparently be completely indigenous and supervised by a committee comprising of members from the Centre for Development of Advanced Computing (C-DAC), Department of Information Technology, IITs including IIT Kanpur, IIT Mumbai, IIT Chennai and IIT Jodhpur, and a few public sector units. The immediate need for tablets, will however be managed by Bharat Electronics Ltd (BEL) and Electronics Corp. of India Ltd.</t>
+  </si>
+  <si>
+    <t>27/02/2012</t>
+  </si>
+  <si>
+    <t>Aakash Put on Notice as BSNL and Pantel Pair up to Produce T-Pad</t>
+  </si>
+  <si>
+    <t>http://www.engadget.com/2012/02/27/BNSL-pantel-aakash-rival/</t>
+  </si>
+  <si>
+    <t>Bharat Sanchar Nigam Limited (BSNL), itself currently under investigation for corruption allegations, has announced a similarly low priced tablet in partnership with Pantel International. The T-Pad IS701R costs Rs 3,250 ($66) compared to the Aakash's Rs 2,999 ($60) but this device has a faster 1GHz processor and runs Gingerbread on a 7-inch 800 x 600 resistive display.</t>
+  </si>
+  <si>
+    <t>09/03/2012</t>
+  </si>
+  <si>
+    <t>DoT Clears Distribution of 50 Lakh Tablet PCs in Schools, Colleges</t>
+  </si>
+  <si>
+    <t>Sandeep Joshi, The Hindu</t>
+  </si>
+  <si>
+    <t>http://www.thehindu.com/sci-tech/technology/gadgets/dot-clears-distribution-of-50-lakh-tablet-pcs-in-schools-colleges/article2975284.ece</t>
+  </si>
+  <si>
+    <t>The DoT has declared that the Centre for Development of Advanced Computing (C-DAC), the research and design wing of the Department of Information Technology, will be the nodal agency for successfully implementing the Aakash-2 project. It will be assisted by the Indian Institute of Technology-Mumbai. They will be responsible for finalising specifications, ensuring quality and testing the tablet PCs. The DoT has decided to rope in two PSUs — Bharat Electronics Ltd and ITI Ltd — for manufacturing and procuring the tablet PCs that will be priced between $55 and $70 (around Rs.2,750 and Rs.3,500).</t>
+  </si>
+  <si>
+    <t>13/04/2012</t>
+  </si>
+  <si>
+    <t>New Twist in Aakash Tablet Controversy</t>
+  </si>
+  <si>
+    <t>Surabhi Agarwal, Live Mint</t>
+  </si>
+  <si>
+    <t>http://www.livemint.com/Companies/tPJizgWhozc5bEVdIenGfL/New-twist-in-Aakash-tablet-controversy.html</t>
+  </si>
+  <si>
+    <t>The controversy over the Indian government’s $45 tablet, Aakash, has taken a fresh twist, with a scrap breaking out between the manufacturer, Canada’s DataWind Ltd, and its erstwhile assembly partner, Hyderabad’s Quad Electronics Solutions Pvt. Ltd... The fight between the two former partners, who have terminated their relationship and claim to have served legal notices to each other, is the latest chapter in the troubled saga of the government’s ambitious effort to bridge the digital divide with a low-cost product.</t>
+  </si>
+  <si>
+    <t>14/04/2012</t>
+  </si>
+  <si>
+    <t>Datawind Breaks Ties with Supplier, Aakash Delayed </t>
+  </si>
+  <si>
+    <t>http://articles.economictimes.indiatimes.com/2012-04-14/news/31342139_1_iit-rajasthan-and-datawind-android-tablets-aakash</t>
+  </si>
+  <si>
+    <t>"Quad circumvented our relationship with IIT-Rajasthan, signed a direct memorandum of understanding with them and then sold off its inventory in the open market," Tuli said... People close to the development said that Datawind is evaluating new manufacturing partners in Noida and Cochin but nothing has been finalized yet.</t>
+  </si>
+  <si>
+    <t>17/04/2012</t>
+  </si>
+  <si>
+    <t>Govt. Accepted 650 Out Of 6440 Tablets; Spat Between DataWind &amp; Quad</t>
+  </si>
+  <si>
+    <t>Anupam Saxena, MediaNama</t>
+  </si>
+  <si>
+    <t>http://www.medianama.com/2012/04/223-aakash-tablet-govt-accepted-650-out-of-6440-tablets-spat-between-datawind-quad/</t>
+  </si>
+  <si>
+    <t>DataWind has said that it has paid Quad for all tablets barring 600, for which it has still not received payment from IIT-Rajasthan, countering Quad’s reported claim that it stopped deliveries to DataWind after 10,000 units due to non-payment. DataWind has now sent a statement stating that it owns the intellectual property rights of Aakash and that Quad had signed a non-disclosure agreement and a manufacturing services agreement with the company, confirming this. The company has alleged that Quad has breached the agreement and sold tablets in the open market. DataWind has also rubbished reports that claim that the Government has not renewed the company’s contract and that it will be supplying 1,00,000 Aakash-2 tablets through IIT-Bombay.</t>
+  </si>
+  <si>
+    <t>23/04/2012</t>
+  </si>
+  <si>
+    <t>Upgraded Aakash Tablet To Be Launched In May; DataWind Vs IIT-Rajasthan</t>
+  </si>
+  <si>
+    <t>http://www.medianama.com/2012/04/223-upgraded-aakash-tablet-to-be-launched-in-may-datawind-vs-iit-rajasthan/</t>
+  </si>
+  <si>
+    <t>n a bid to ‘clear the air’ around the controversial Aakash tablet project, DataWind, the company that had won the contract for manufacturing the tablet for the Indian government, informed that following the transfer of the project from IIT-Rajasthan to IIT-Bombay, the latter is issuing a purchase order for 1,00,000 upgraded Aakash tablets, which DataWind intends to deliver by May. DataWind CEO, Suneet Singh Tuli, said that the government will launch the upgraded Aakash tablet device in May upon approval of the initial deliveries, for which IIT-Bombay and C-DAC (Centre for Development of Advanced Computing) will be conducting testing and certification, at the same price.</t>
+  </si>
+  <si>
+    <t>27/04/2012</t>
+  </si>
+  <si>
+    <t>The Tangled Tale of Aakash, the World’s Cheapest Laptop</t>
+  </si>
+  <si>
+    <t>http://india.blogs.nytimes.com/2012/04/27/the-tangled-tale-of-aakash-the-worlds-cheapest-laptop/</t>
+  </si>
+  <si>
+    <t>I.I.T. Rajasthan is no longer involved, having been replaced by I.I.T. Bombay. DataWind and the company’s India-based subcontractor, Quad Electronic, are having a financial dispute: Quad Electronic claims DataWind owes it $1.12 million, which DataWind denies. Meanwhile, I.I.T. Rajasthan is claiming damages of nearly half a million dollars from DataWind, while DataWind says I.I.T. Rajathan did not return its bid deposit of nearly $100,000. Oh, and DataWind has sent a legal notice to the Indian Cellular Association, accusing them of defamation.</t>
+  </si>
+  <si>
+    <t>30/04/2012</t>
+  </si>
+  <si>
+    <t>The Aakash Project’s Bitter Finish</t>
+  </si>
+  <si>
+    <t>http://india.blogs.nytimes.com/2012/04/30/the-aakash-projects-bitter-finish/</t>
+  </si>
+  <si>
+    <t>In late February, a committee headed by R. Chandrashekhar, a senior bureaucrat in the government’s Information and technology department, met to discuss the project. In the weeks that followed, the government decided that the project should be transferred from I.I.T. Rajasthan to I.I.T. Bombay, with the consent of the director of I.I.T. Rajasthan, Mr. Kalra. Aakash is now being led by Deepak B. Phatak, a professor at I.I.T. Bombay, who set up the Affordable Solutions Lab in 2003, which aims to develop low-cost technological solutions.</t>
+  </si>
+  <si>
+    <t>21/05/2012</t>
+  </si>
+  <si>
+    <t>Cloudy Outlook for Aakash</t>
+  </si>
+  <si>
+    <t>Ashok Parthasarathi, The Hindu</t>
+  </si>
+  <si>
+    <t>http://www.thehindu.com/opinion/op-ed/article3439629.ece</t>
+  </si>
+  <si>
+    <t>Mr. Sibal announced in Parliament recently that DWL had since ceased its collaboration with IIT Rajasthan and will now be supplying the one lakh “Aakash” Tablets in collaboration with IIT Bombay! This appears to be in total contradiction of what he told the media on the sidelines of the inauguration of the World IT Forum 2012 on April 17. He said, “We have invited companies from across the world for manufacturing and many are ready to manufacture it here. Currently we are looking at the design and other parameters. After we freeze the design and technology, manufacturing will take place.” More astonishingly, despite the huge work agenda listed by Mr. Sibal, he has concluded in Parliament that “the second version of ‘Aakash' will be launched in May!”</t>
+  </si>
+  <si>
+    <t>23/05/2012</t>
+  </si>
+  <si>
+    <t>Aakash Tablet RTI: Rs 47.72 Cr For 100,000 Tabs, Cost $49.98 Each; No Tender Docs With Ministry</t>
+  </si>
+  <si>
+    <t>Nikhil Pahwa, MediaNama</t>
+  </si>
+  <si>
+    <t>http://www.medianama.com/2012/05/223-aakash-tablet-rti-rs-47-72-cr-for-100000-tabs-cost-49-98-each-no-tender-docs-with-ministry/</t>
+  </si>
+  <si>
+    <t>The HRD Ministry has released Rs 47.72 crore to IIT Rajasthan for testing low cost access-cum-computing devices and hardware and software optimization of low cost access devices. The ministry says that it does not have details of the tender/document/financial bid/payment made by IIT Rajasthan to Datawind... The HRD Ministry says that it has no information regarding the number of tablets provided to IIT Rajasthan by Datawind, the list of educational institutions to which Aakash Tablets have been distributed, the total number of tablets that have been issued and how many students in each educational institution have been issued the Aakash Tablet.</t>
+  </si>
+  <si>
+    <t>28/05/2012</t>
+  </si>
+  <si>
+    <t>Aakash Tablet RTI: Only 572 Tablets Distributed To 19 Colleges</t>
+  </si>
+  <si>
+    <t>http://www.medianama.com/2012/05/223-aakash-tablet-rti-college-datawind/</t>
+  </si>
+  <si>
+    <t>IIT Rajasthan has so far distributed 572 of the 6640 Aakash Tablet devices received by it from its manufacturer Datawind, the college has said, in response to a Right To Information request filed by MediaNama. Of these, IIT Rajasthan 546 have been distributed to students, while 26 have been distributed to coordinators. IIT Rajasthan itself is the largest recipient of the Aakash Table, with 181 devices having been distributed to students, while Dayalbagh Educational Institute in Agra has received 59 and IIIT-DM in Jabalpur has received 47 devices.</t>
+  </si>
+  <si>
+    <t>02/06/2012</t>
+  </si>
+  <si>
+    <t>Aakash 2, the Cheapest Tablet PC, Misses May-End Deadline</t>
+  </si>
+  <si>
+    <t>http://articles.economictimes.indiatimes.com/2012-06-02/news/31984185_1_tablet-datawind-kapil-sibal</t>
+  </si>
+  <si>
+    <t> Datawind ended the relationship with Hyderabad-based Quad Electronics, its Indian manufacturing partner, causing delays in the supply of tablets. Datawind was supposed to supply 1,00,000 tablets to IIT-Rajasthan. Since then, Datawind has contracted Hyderabad-based VMC Systems to supply the tablets. About 50 people have reportedly been poached by VMC Systems from Quad Electronics who were earlier working on the Aakash assembly line.</t>
+  </si>
+  <si>
+    <t>18/06/2012</t>
+  </si>
+  <si>
+    <t>How The Failed Aakash Tablet Is An Object Lesson In India's Long Road Ahead To Tech Innovation</t>
+  </si>
+  <si>
+    <t>April Rabkin, Fast Company</t>
+  </si>
+  <si>
+    <t>http://www.fastcompany.com/1839297/how-failed-aakash-tablet-object-lesson-indias-long-road-ahead-tech-innovation</t>
+  </si>
+  <si>
+    <t>Throughout the month, hundreds of Aakashes began to arrive at IIT Rajasthan for testing. The problems were immediately evident. According to one source close to the university, a third of the devices didn't start at all. Most of those that did either failed the basic drop test, overheated quickly, or saw their screens freeze until the battery ran out. A peek inside the box revealed circuitry and imported components held together by electrical tape.</t>
+  </si>
+  <si>
+    <t>19/09/2012</t>
+  </si>
+  <si>
+    <t>India Proposes JV with Turkmenistan to Manufacture Aakash</t>
+  </si>
+  <si>
+    <t>Satrapia</t>
+  </si>
+  <si>
+    <t>http://www.satrapia.com/news/article/india-proposes-jv-with-turkmenistan-to-manufacture-aakash/</t>
+  </si>
+  <si>
+    <t>Indian telecom Minister Kapil Sibal, who is on a visit to Turkmenistan, suggested forming a joint venture company which may manufacture Aakash, according to an official release. Indian side will design the necessary hardware and software of the tablet fulfilling the Turkmen side needs, it added. “Besides supplying the low-cost tablets, the joint venture company can market the product to other international markets,” he said. </t>
+  </si>
+  <si>
+    <t>22/10/2012</t>
+  </si>
+  <si>
+    <t>Ministers Give Thumbs up to Aakash II</t>
+  </si>
+  <si>
+    <t>Business Line</t>
+  </si>
+  <si>
+    <t>http://www.thehindubusinessline.com/industry-and-economy/info-tech/ministers-give-thumbs-up-to-aakashii/article4022563.ece</t>
+  </si>
+  <si>
+    <t> The new version of Aakash has been given a positive rating by Union ministers, whose feedback on the low cost computing device were sought, with the Labour Ministry proposing to provide it in ITIs also. Aakash-II tablets, which will be officially launched by President Pranab Mukherjee here on education day on November 11, were sent to all ministers as well as state chief ministers for their views and suggestions.</t>
+  </si>
+  <si>
+    <t>09/11/2012</t>
+  </si>
+  <si>
+    <t>We have made many mistakes, but I've left them behind: Datawind CEO</t>
+  </si>
+  <si>
+    <t>S. Ronendra Singh, The Hindu</t>
+  </si>
+  <si>
+    <t>http://www.thehindubusinessline.com/industry-and-economy/info-tech/we-have-made-many-mistakes-but-ive-left-them-behind-datawind-ceo/article4081841.ece</t>
+  </si>
+  <si>
+    <t>We helped create a market of Rs 6,500–7,000 a tablet that cost Rs 15,000–20,000 a year ago by companies such as Micromax and Lava. We are selling our product at Rs 2,263 to the Government and for Rs 3,500 to the consumers. Computing/ Internet has arrived in India, which could leave behind the telecom revolution... We are getting a margin of less than 10 per cent from the Government deal and around 15 per cent from the consumers, but we do not mind that. </t>
+  </si>
+  <si>
+    <t>11/12/2012</t>
+  </si>
+  <si>
+    <t>President Unveils Aakash Version 2.0 Tablet on National Education Day</t>
+  </si>
+  <si>
+    <t>http://pib.nic.in/newsite/PrintRelease.aspx?relid=88984</t>
+  </si>
+  <si>
+    <t>The President of India, Shri Pranab Mukherjee took the occasion of National Education Day to release and dedicate to the nation, the innovative and modestly-priced Aakash Version 2.0 tablet in New Delhi today... Aakash Version 2.0 is a full-fledged tablet computer. IIT Bombay along with the Ministry of Human Resource Development has created several useful educational applications for the tablet. Teachers and students in the remotest corners of India can join a classroom and benefit from lectures delivered by the best teachers. </t>
+  </si>
+  <si>
+    <t>14/11/2012</t>
+  </si>
+  <si>
+    <t>Indian Government Unveils Aakash 2 Tablet; Aakash In Education</t>
+  </si>
+  <si>
+    <t>http://www.medianama.com/2012/11/223-indian-government-unveils-aakash-2-tablet-aakash-in-education/</t>
+  </si>
+  <si>
+    <t>Similar to the original Aakash, this Android based tablet has been designed, developed and manufactured by Datawind for supply to IIT Bombay, under the HRD Ministry’s National Mission on Education through Information &amp; Communication Technology (NME-ICT)... According to the press statement, Datawind will be providing 100,000 units of Aakash 2 to IIT Bombay in the first phase, which in turn intends to distribute these tablets to Engineering students across various colleges and universities. The government intends to distribute these tablets to over 220 million Indian students in the coming years.</t>
+  </si>
+  <si>
+    <t>18/11/2012</t>
+  </si>
+  <si>
+    <t>Datawind to Clear All Paid Orders for Aakash in 6 Weeks</t>
+  </si>
+  <si>
+    <t>http://www.thehindubusinessline.com/industry-and-economy/info-tech/datawind-to-clear-all-paid-orders-for-aakash-in-6-weeks/article4108396.ece</t>
+  </si>
+  <si>
+    <t>“All the paid orders (for tablets with) resistive and capacitative (screens) without SIM will be cleared in next 10 days. But the ones that want tablet with SIM will be cleared in 4 to 6 weeks,” DataWind CEO Suneet Singh Tuli told PTI. </t>
+  </si>
+  <si>
+    <t>24/11/2012</t>
+  </si>
+  <si>
+    <t>Conned: Aakash 2 made in China?</t>
+  </si>
+  <si>
+    <t>Vivek Sinha, Hindustan Times</t>
+  </si>
+  <si>
+    <t>http://www.hindustantimes.com/technology/gadgets-updates/conned-aakash-2-made-in-china/article1-963600.aspx</t>
+  </si>
+  <si>
+    <t>Documents reviewed by HT show DataWind founders and NRI brothers Suneet and Raja Singh Tuli may have procured these devices off-the-shelf from manufacturers in China for $42 ( Rs. 2,263 then), exactly the price at which they sold these to the Indian government. DataWind bought more than 10,000 or more "A 13" made-in-China tablets from at least four manufacturers in Shenzhen and Hong Kong between October 26 and November 7. These were shipped to India duty-free as they were meant for school students under an HRD ministry programme.</t>
+  </si>
+  <si>
+    <t>26/11/2012</t>
+  </si>
+  <si>
+    <t>India’s ‘Aakash,’ Now Made in China</t>
+  </si>
+  <si>
+    <t>Pamposh Raina and Mia Li, The New York Times</t>
+  </si>
+  <si>
+    <t>http://india.blogs.nytimes.com/2012/11/26/india%E2%80%99s-super-cheap-tablet-now-made-in-china/?_php=true&amp;_type=blogs&amp;_php=true&amp;_type=blogs&amp;_r=1</t>
+  </si>
+  <si>
+    <t>DataWind, the Canada-based company that won a government contract to produce the first 100,000 Aakash tablets, which are bound for India’s colleges and universities, “does only sales,” said Li Junhao, the president of Trend Grace, a company based in Shenzhen that is one of several Chinese manufacturers making Aakash-2 tablets, according to invoices sent to DataWind that were reviewed by India Ink. “The tablets we sell to DataWind are ready to be sold. They are finished, ready-to-use products,” Mr. Li said in a telephone interview.</t>
+  </si>
+  <si>
+    <t>27/11/2012</t>
+  </si>
+  <si>
+    <t>Updated: Aakash 2 Manufactured In China And Not India: Report; Datawind Refutes Allegations</t>
+  </si>
+  <si>
+    <t>Apurva Chaudhary, MediaNama</t>
+  </si>
+  <si>
+    <t>http://www.medianama.com/2012/11/223-aakash-2-manufactured-in-china-and-not-india-report-datawind-refutes-allegations/</t>
+  </si>
+  <si>
+    <t>Datawind sold these tablets to the government exactly at the same price at which they procured them. The tablet is being distributed to students by Datawind at government subsidized cost of Rs 1,130. Documents reviewed by HT show that Datawind bought more than 10,000 tablets made in China from four manufacturers in Shenzhen and Hong Kong — Kalong Technology Co., Ltd, Dasen International Electronics Co Ltd, Trend Grace and Shenzhen Shetong Zhaoli Co Ltd... IIT-Bombay had issued a certificate dated October 29 for importing about 20,000 tablets into India.</t>
+  </si>
+  <si>
+    <t>Dear Mr Tuli, We’d be Grateful if You could Start Shipping - An Open Letter to Datawind CEO</t>
+  </si>
+  <si>
+    <t>Jayadevan P.K., NextBigWhat</t>
+  </si>
+  <si>
+    <t>http://www.nextbigwhat.com/open-letter-to-sunit-tuli-datawind-297/</t>
+  </si>
+  <si>
+    <t>If you seriously believe that those “allegations are a desperate attempt sabotage the image of India,” we wish that you would remain unfazed by the allegations levelled at your firm by a certain newspaper and start shipping now. Be sure to get rid of those “misleading” labels. Never mind that subsequently, another reporter dug out documents showing that about 12,000 devices designed by AllWinner Tech of China were procured by your company Datawind weeks before the launch date on November 11. For all you know, it could be Chinese propaganda.</t>
+  </si>
+  <si>
+    <t>29/11/2012</t>
+  </si>
+  <si>
+    <t>Aakash 2 Tablet Unveiled at UN Headquarters</t>
+  </si>
+  <si>
+    <t>http://articles.economictimes.indiatimes.com/2012-11-29/news/35433152_1_aakash-tablet-suneet-singh-tuli-datawind</t>
+  </si>
+  <si>
+    <t> UN Secretary General Ban Ki-moon praised India as a "super-power" in the field of information technology as he unveiled the country's first indigenously created low-cost Aakash 2 tablet here. The tablet was showcased at the UN headquarters yesterday on the occasion of the India's current Presidency of the UN Security Council.</t>
+  </si>
+  <si>
+    <t>30/11/2012</t>
+  </si>
+  <si>
+    <t>The Storm behind DataWind’s Aakash Tablets</t>
+  </si>
+  <si>
+    <t>Rajesh Kurup, Business Line</t>
+  </si>
+  <si>
+    <t>http://www.thehindubusinessline.com/industry-and-economy/info-tech/the-storm-behind-datawinds-aakash-tablets/article4151110.ece</t>
+  </si>
+  <si>
+    <t>“Although we are big proponents of manufacturing in India, and there are significant efforts to enable numerous manufacturers to be able to produce tablets in India, there was no commitment to make the product in India,” DataWind Chief Executive Officer Suneet Singh Tuli said in an e-mail reply to Business Line. The box of the Ubislate series tablets manufactured by DataWind also did not mention that the devices were ‘Made in India’, he said. </t>
+  </si>
+  <si>
+    <t>10/11/2012</t>
+  </si>
+  <si>
+    <t>Priyamani to Endorse Aakash 2 Tablet?</t>
+  </si>
+  <si>
+    <t>KollyTalk</t>
+  </si>
+  <si>
+    <t>http://www.kollytalk.com/cinenews/priyamani-to-endorse-aakash-2-tablet-75009.html</t>
+  </si>
+  <si>
+    <t>The actress mentioned, “I have not yet signed on any papers regarding the Aakash deal yet. But I am in talks with the concerned authorities and would like to be part of my first deal as a brand ambassador”.</t>
   </si>
 </sst>
 </file>
@@ -469,7 +985,7 @@
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="@" numFmtId="165"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -494,6 +1010,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <b val="true"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="000000FF"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -539,15 +1061,21 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -567,123 +1095,123 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="true" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <pane activePane="bottomRight" topLeftCell="B51" xSplit="1" ySplit="1"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
       <selection activeCell="B1" activeCellId="0" pane="topRight" sqref="B1"/>
-      <selection activeCell="A2" activeCellId="0" pane="bottomLeft" sqref="A2"/>
-      <selection activeCell="C3" activeCellId="0" pane="bottomRight" sqref="C3"/>
+      <selection activeCell="A51" activeCellId="0" pane="bottomLeft" sqref="A51"/>
+      <selection activeCell="F68" activeCellId="0" pane="bottomRight" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.7176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9725490196078"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.5372549019608"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="32.7137254901961"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="51.3803921568628"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="15.9725490196078"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="17.5372549019608"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="32.7137254901961"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="51.3803921568628"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="2" width="11.5764705882353"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.5" outlineLevel="0" r="1" s="2">
-      <c r="A1" s="2" t="s">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.5" outlineLevel="0" r="1" s="4">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.2" outlineLevel="0" r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.2" outlineLevel="0" r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="69.25" outlineLevel="0" r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="46.55" outlineLevel="0" r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -691,19 +1219,19 @@
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -711,19 +1239,19 @@
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -731,19 +1259,19 @@
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -751,99 +1279,99 @@
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="125.95" outlineLevel="0" r="10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="80.55" outlineLevel="0" r="11">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="125.95" outlineLevel="0" r="12">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="91.9" outlineLevel="0" r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -851,239 +1379,239 @@
       <c r="A14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="69.25" outlineLevel="0" r="15">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="103.25" outlineLevel="0" r="16">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="114.6" outlineLevel="0" r="17">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="137.3" outlineLevel="0" r="18">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="125.95" outlineLevel="0" r="19">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="125.95" outlineLevel="0" r="20">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="103.25" outlineLevel="0" r="21">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="91.9" outlineLevel="0" r="22">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="103.25" outlineLevel="0" r="23">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="80.55" outlineLevel="0" r="24">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="91.9" outlineLevel="0" r="25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1091,19 +1619,19 @@
       <c r="A26" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1111,19 +1639,19 @@
       <c r="A27" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1131,39 +1659,39 @@
       <c r="A28" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="149.25" outlineLevel="0" r="29">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1171,19 +1699,19 @@
       <c r="A30" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1191,23 +1719,802 @@
       <c r="A31" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="69.25" outlineLevel="0" r="32">
+      <c r="A32" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="91.9" outlineLevel="0" r="33">
+      <c r="A33" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="114.6" outlineLevel="0" r="34">
+      <c r="A34" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="80.55" outlineLevel="0" r="35">
+      <c r="A35" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.9" outlineLevel="0" r="36">
+      <c r="A36" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="125.95" outlineLevel="0" r="37">
+      <c r="A37" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="125.95" outlineLevel="0" r="38">
+      <c r="A38" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="114.6" outlineLevel="0" r="39">
+      <c r="A39" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="91.9" outlineLevel="0" r="40">
+      <c r="A40" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="160.55" outlineLevel="0" r="41">
+      <c r="A41" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="125.95" outlineLevel="0" r="42">
+      <c r="A42" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="80.55" outlineLevel="0" r="43">
+      <c r="A43" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="125.95" outlineLevel="0" r="44">
+      <c r="A44" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="103.25" outlineLevel="0" r="45">
+      <c r="A45" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="69.25" outlineLevel="0" r="46">
+      <c r="A46" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="160.55" outlineLevel="0" r="47">
+      <c r="A47" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="149.25" outlineLevel="0" r="48">
+      <c r="A48" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="114.6" outlineLevel="0" r="49">
+      <c r="A49" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="114.6" outlineLevel="0" r="50">
+      <c r="A50" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="160.55" outlineLevel="0" r="51">
+      <c r="A51" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="137.3" outlineLevel="0" r="52">
+      <c r="A52" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="114.6" outlineLevel="0" r="53">
+      <c r="A53" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="91.9" outlineLevel="0" r="54">
+      <c r="A54" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="91.9" outlineLevel="0" r="55">
+      <c r="A55" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="91.9" outlineLevel="0" r="56">
+      <c r="A56" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="91.9" outlineLevel="0" r="57">
+      <c r="A57" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="91.9" outlineLevel="0" r="58">
+      <c r="A58" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="114.6" outlineLevel="0" r="59">
+      <c r="A59" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="125.95" outlineLevel="0" r="60">
+      <c r="A60" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="46.55" outlineLevel="0" r="61">
+      <c r="A61" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="114.6" outlineLevel="0" r="62">
+      <c r="A62" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="114.6" outlineLevel="0" r="63">
+      <c r="A63" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="114.6" outlineLevel="0" r="64">
+      <c r="A64" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="114.6" outlineLevel="0" r="65">
+      <c r="A65" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="69.25" outlineLevel="0" r="66">
+      <c r="A66" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="91.9" outlineLevel="0" r="67">
+      <c r="A67" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="46.55" outlineLevel="0" r="68">
+      <c r="A68" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink display="http://articles.economictimes.indiatimes.com/2012-01-03/news/30584606_1_aakash-tablets-indian-tablet-market-current-tablet" ref="D32" r:id="rId1"/>
+    <hyperlink display="http://indiatoday.intoday.in/story/kapil-sibal-cheapest-tablet-of-world-aakash-failure/1/167730.html" ref="D33" r:id="rId2"/>
+    <hyperlink display="http://indiatoday.intoday.in/story/aakash-low-cost-india-tablet-kapil-sibal/1/168564.html" ref="D34" r:id="rId3"/>
+    <hyperlink display="http://timesofindia.indiatimes.com/tech/tech-news/Aakash-tablet-Datawind-opposes-IITs-test-standard/articleshow/11508146.cms" ref="D35" r:id="rId4"/>
+    <hyperlink display="http://www.themobileindian.com/news/4811_Aakash-loses-government-edge" ref="D36" r:id="rId5"/>
+    <hyperlink display="http://spectrum.ieee.org/geek-life/tools-toys/searching-for-the-aakash" ref="D37" r:id="rId6"/>
+    <hyperlink display="http://articles.economictimes.indiatimes.com/2012-02-02/news/31017361_1_aakash2-iit-rajasthan-tablets" ref="D38" r:id="rId7"/>
+    <hyperlink display="http://truthdive.com/2012/02/03/aakash-tablet-3-more-iits-to-work-for-making-it-cheaper.html" ref="D39" r:id="rId8"/>
+    <hyperlink display="http://www.engadget.com/2012/02/22/aakash-stalls/" ref="D40" r:id="rId9"/>
+    <hyperlink display="http://www.mydigitalfc.com/op-ed/clouds-doubt-over-aakash-680" ref="D41" r:id="rId10"/>
+    <hyperlink display="http://www.medianama.com/2012/02/223-aakash-tablet-project-govt-dumps-datawind-medianamas-rti/" ref="D42" r:id="rId11"/>
+    <hyperlink display="http://www.engadget.com/2012/02/27/BNSL-pantel-aakash-rival/" ref="D43" r:id="rId12"/>
+    <hyperlink display="http://www.thehindu.com/sci-tech/technology/gadgets/dot-clears-distribution-of-50-lakh-tablet-pcs-in-schools-colleges/article2975284.ece" ref="D44" r:id="rId13"/>
+    <hyperlink display="http://www.livemint.com/Companies/tPJizgWhozc5bEVdIenGfL/New-twist-in-Aakash-tablet-controversy.html" ref="D45" r:id="rId14"/>
+    <hyperlink display="http://articles.economictimes.indiatimes.com/2012-04-14/news/31342139_1_iit-rajasthan-and-datawind-android-tablets-aakash" ref="D46" r:id="rId15"/>
+    <hyperlink display="http://www.medianama.com/2012/04/223-aakash-tablet-govt-accepted-650-out-of-6440-tablets-spat-between-datawind-quad/" ref="D47" r:id="rId16"/>
+    <hyperlink display="http://www.medianama.com/2012/04/223-upgraded-aakash-tablet-to-be-launched-in-may-datawind-vs-iit-rajasthan/" ref="D48" r:id="rId17"/>
+    <hyperlink display="http://india.blogs.nytimes.com/2012/04/27/the-tangled-tale-of-aakash-the-worlds-cheapest-laptop/" ref="D49" r:id="rId18"/>
+    <hyperlink display="http://india.blogs.nytimes.com/2012/04/30/the-aakash-projects-bitter-finish/" ref="D50" r:id="rId19"/>
+    <hyperlink display="http://www.thehindu.com/opinion/op-ed/article3439629.ece" ref="D51" r:id="rId20"/>
+    <hyperlink display="http://www.medianama.com/2012/05/223-aakash-tablet-rti-rs-47-72-cr-for-100000-tabs-cost-49-98-each-no-tender-docs-with-ministry/" ref="D52" r:id="rId21"/>
+    <hyperlink display="http://www.medianama.com/2012/05/223-aakash-tablet-rti-college-datawind/" ref="D53" r:id="rId22"/>
+    <hyperlink display="http://articles.economictimes.indiatimes.com/2012-06-02/news/31984185_1_tablet-datawind-kapil-sibal" ref="D54" r:id="rId23"/>
+    <hyperlink display="http://www.fastcompany.com/1839297/how-failed-aakash-tablet-object-lesson-indias-long-road-ahead-tech-innovation" ref="D55" r:id="rId24"/>
+    <hyperlink display="http://www.satrapia.com/news/article/india-proposes-jv-with-turkmenistan-to-manufacture-aakash/" ref="D56" r:id="rId25"/>
+    <hyperlink display="http://www.thehindubusinessline.com/industry-and-economy/info-tech/ministers-give-thumbs-up-to-aakashii/article4022563.ece" ref="D57" r:id="rId26"/>
+    <hyperlink display="http://www.thehindubusinessline.com/industry-and-economy/info-tech/we-have-made-many-mistakes-but-ive-left-them-behind-datawind-ceo/article4081841.ece" ref="D58" r:id="rId27"/>
+    <hyperlink display="http://pib.nic.in/newsite/PrintRelease.aspx?relid=88984" ref="D59" r:id="rId28"/>
+    <hyperlink display="http://www.medianama.com/2012/11/223-indian-government-unveils-aakash-2-tablet-aakash-in-education/" ref="D60" r:id="rId29"/>
+    <hyperlink display="http://www.thehindubusinessline.com/industry-and-economy/info-tech/datawind-to-clear-all-paid-orders-for-aakash-in-6-weeks/article4108396.ece" ref="D61" r:id="rId30"/>
+    <hyperlink display="http://www.hindustantimes.com/technology/gadgets-updates/conned-aakash-2-made-in-china/article1-963600.aspx" ref="D62" r:id="rId31"/>
+    <hyperlink display="http://india.blogs.nytimes.com/2012/11/26/india%E2%80%99s-super-cheap-tablet-now-made-in-china/?_php=true&amp;_type=blogs&amp;_php=true&amp;_type=blogs&amp;_r=1" ref="D63" r:id="rId32"/>
+    <hyperlink display="http://www.medianama.com/2012/11/223-aakash-2-manufactured-in-china-and-not-india-report-datawind-refutes-allegations/" ref="D64" r:id="rId33"/>
+    <hyperlink display="http://www.nextbigwhat.com/open-letter-to-sunit-tuli-datawind-297/" ref="D65" r:id="rId34"/>
+    <hyperlink display="http://articles.economictimes.indiatimes.com/2012-11-29/news/35433152_1_aakash-tablet-suneet-singh-tuli-datawind" ref="D66" r:id="rId35"/>
+    <hyperlink display="http://www.thehindubusinessline.com/industry-and-economy/info-tech/the-storm-behind-datawinds-aakash-tablets/article4151110.ece" ref="D67" r:id="rId36"/>
+    <hyperlink display="http://www.kollytalk.com/cinenews/priyamani-to-endorse-aakash-2-tablet-75009.html" ref="D68" r:id="rId37"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>

</xml_diff>